<commit_message>
Updated Work for First Video Presentation
</commit_message>
<xml_diff>
--- a/Data Files for Python/Summary Statistics for Automotive Data.xlsx
+++ b/Data Files for Python/Summary Statistics for Automotive Data.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
   <si>
     <t>symboling</t>
   </si>
@@ -452,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,10 +519,13 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>201</v>
@@ -549,11 +555,11 @@
         <v>201</v>
       </c>
       <c r="K2">
+        <v>201</v>
+      </c>
+      <c r="L2">
         <v>197</v>
       </c>
-      <c r="L2">
-        <v>201</v>
-      </c>
       <c r="M2">
         <v>201</v>
       </c>
@@ -578,438 +584,462 @@
       <c r="T2">
         <v>201</v>
       </c>
+      <c r="U2">
+        <v>201</v>
+      </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
         <v>0.8407960199004975</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>122</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>98.79701492537313</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.8371023307298204</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.9151257600884466</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>53.76666666666667</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>2555.666666666667</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>126.8756218905473</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>3.33069156704042</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>3.256903553299492</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>10.16427860696517</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>103.4055339068206</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>5117.665367742568</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>25.17910447761194</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>30.68656716417911</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>13207.12935323383</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>9.944145483678392</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>0.09950248756218906</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>0.900497512437811</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4">
+        <v>58.16786054171152</v>
+      </c>
+      <c r="C4">
         <v>1.25480172265744</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>31.99624978024768</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>6.066365554825733</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.05921275873275769</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.02918709470463724</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2.447822161296309</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>517.2967265828513</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>41.54683444904459</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.2680718571228559</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.3192562399907384</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>4.004965493233374</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>37.36569950210651</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>478.1138050197773</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>6.423220469050541</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>6.815149936480959</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>7947.066341939274</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>2.534599261240003</v>
-      </c>
-      <c r="S4">
-        <v>0.3000829072836058</v>
       </c>
       <c r="T4">
         <v>0.3000829072836058</v>
       </c>
+      <c r="U4">
+        <v>0.3000829072836058</v>
+      </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>-2</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>65</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>86.59999999999999</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.6780394041326285</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.8374999999999999</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>47.8</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1488</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>61</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>2.54</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>2.07</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>7</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>48</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>4150</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>13</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>16</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>5118</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>4.795918367346938</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
       </c>
       <c r="T5">
         <v>0</v>
       </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>101</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>94.5</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.8015377222489188</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.8902777777777777</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>52</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>2169</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>98</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>3.15</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>3.11</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>8.6</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>70</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>4800</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>19</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>25</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>7775</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>7.833333333333332</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>0</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>122</v>
+      </c>
+      <c r="E7">
+        <v>97</v>
+      </c>
+      <c r="F7">
+        <v>0.8322921672272945</v>
+      </c>
+      <c r="G7">
+        <v>0.9097222222222222</v>
+      </c>
+      <c r="H7">
+        <v>54.1</v>
+      </c>
+      <c r="I7">
+        <v>2414</v>
+      </c>
+      <c r="J7">
+        <v>120</v>
+      </c>
+      <c r="K7">
+        <v>3.31</v>
+      </c>
+      <c r="L7">
+        <v>3.29</v>
+      </c>
+      <c r="M7">
+        <v>9</v>
+      </c>
+      <c r="N7">
+        <v>95</v>
+      </c>
+      <c r="O7">
+        <v>5125.369458128079</v>
+      </c>
+      <c r="P7">
         <v>24</v>
       </c>
-      <c r="B7">
+      <c r="Q7">
+        <v>30</v>
+      </c>
+      <c r="R7">
+        <v>10295</v>
+      </c>
+      <c r="S7">
+        <v>9.791666666666666</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
         <v>1</v>
       </c>
-      <c r="C7">
-        <v>122</v>
-      </c>
-      <c r="D7">
-        <v>97</v>
-      </c>
-      <c r="E7">
-        <v>0.8322921672272945</v>
-      </c>
-      <c r="F7">
-        <v>0.9097222222222222</v>
-      </c>
-      <c r="G7">
-        <v>54.1</v>
-      </c>
-      <c r="H7">
-        <v>2414</v>
-      </c>
-      <c r="I7">
-        <v>120</v>
-      </c>
-      <c r="J7">
-        <v>3.31</v>
-      </c>
-      <c r="K7">
-        <v>3.29</v>
-      </c>
-      <c r="L7">
-        <v>9</v>
-      </c>
-      <c r="M7">
-        <v>95</v>
-      </c>
-      <c r="N7">
-        <v>5125.369458128079</v>
-      </c>
-      <c r="O7">
-        <v>24</v>
-      </c>
-      <c r="P7">
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>150</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>137</v>
+      </c>
+      <c r="E8">
+        <v>102.4</v>
+      </c>
+      <c r="F8">
+        <v>0.8817876021143681</v>
+      </c>
+      <c r="G8">
+        <v>0.925</v>
+      </c>
+      <c r="H8">
+        <v>55.5</v>
+      </c>
+      <c r="I8">
+        <v>2926</v>
+      </c>
+      <c r="J8">
+        <v>141</v>
+      </c>
+      <c r="K8">
+        <v>3.58</v>
+      </c>
+      <c r="L8">
+        <v>3.41</v>
+      </c>
+      <c r="M8">
+        <v>9.4</v>
+      </c>
+      <c r="N8">
+        <v>116</v>
+      </c>
+      <c r="O8">
+        <v>5500</v>
+      </c>
+      <c r="P8">
         <v>30</v>
       </c>
-      <c r="Q7">
-        <v>10295</v>
-      </c>
-      <c r="R7">
-        <v>9.791666666666666</v>
-      </c>
-      <c r="S7">
+      <c r="Q8">
+        <v>34</v>
+      </c>
+      <c r="R8">
+        <v>16500</v>
+      </c>
+      <c r="S8">
+        <v>12.36842105263158</v>
+      </c>
+      <c r="T8">
         <v>0</v>
       </c>
-      <c r="T7">
+      <c r="U8">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>137</v>
-      </c>
-      <c r="D8">
-        <v>102.4</v>
-      </c>
-      <c r="E8">
-        <v>0.8817876021143681</v>
-      </c>
-      <c r="F8">
-        <v>0.925</v>
-      </c>
-      <c r="G8">
-        <v>55.5</v>
-      </c>
-      <c r="H8">
-        <v>2926</v>
-      </c>
-      <c r="I8">
-        <v>141</v>
-      </c>
-      <c r="J8">
-        <v>3.58</v>
-      </c>
-      <c r="K8">
-        <v>3.41</v>
-      </c>
-      <c r="L8">
-        <v>9.4</v>
-      </c>
-      <c r="M8">
-        <v>116</v>
-      </c>
-      <c r="N8">
-        <v>5500</v>
-      </c>
-      <c r="O8">
-        <v>30</v>
-      </c>
-      <c r="P8">
-        <v>34</v>
-      </c>
-      <c r="Q8">
-        <v>16500</v>
-      </c>
-      <c r="R8">
-        <v>12.36842105263158</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>256</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>120.9</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>59.8</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>4066</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>326</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>3.94</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>4.17</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>23</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>262</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>6600</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>49</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>54</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>45400</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>18.07692307692308</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>1</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>1</v>
       </c>
     </row>

</xml_diff>